<commit_message>
Filled in peripheral map a little more
</commit_message>
<xml_diff>
--- a/hdw/Logic_Board/Design_Files/Microcontroller_Peripheral_Map.xlsx
+++ b/hdw/Logic_Board/Design_Files/Microcontroller_Peripheral_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Electronic_Display\hdw\Logic_Board\Design_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F1DB2-F654-441C-85A0-756B51C0E0EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFA7EAE-7BBB-4BE9-8B95-A277318D64F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" xr2:uid="{B7D91EF5-14DE-4003-8C97-5F77E28EC198}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Peripheral Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Seiral Peripheral Interface 3</t>
   </si>
   <si>
-    <t>Allows data to be stored and retrieved from external serial FLASH memory</t>
-  </si>
-  <si>
     <t>Software Naming</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Universal Asynchronous Recevier Transmitter 1</t>
   </si>
   <si>
-    <t>Serial connection for WIFI module</t>
-  </si>
-  <si>
     <t>WIFI_UART</t>
   </si>
   <si>
@@ -81,13 +75,49 @@
     <t>Universal Asynchronous Recevier Transmitter 6</t>
   </si>
   <si>
-    <t>Serial connection for USB debugging</t>
-  </si>
-  <si>
     <t>USB_UART</t>
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>WDT</t>
+  </si>
+  <si>
+    <t>Watchdog Timer</t>
+  </si>
+  <si>
+    <t>watchdogTimer</t>
+  </si>
+  <si>
+    <t>Allows data to be stored and retrieved from external serial FLASH memory. There are 8 FLASH chips which each hold a slide of data for the display</t>
+  </si>
+  <si>
+    <t>Serial connection for WIFI module, used for moving image data from an android app into the embedded system</t>
+  </si>
+  <si>
+    <t>Serial connection for USB debugging, virtual COM port</t>
+  </si>
+  <si>
+    <t>Error catch, resets the microcontroller if the timer has not been cleared in 2 seconds. Timer is cleared within the heartbeat ISR (below)</t>
+  </si>
+  <si>
+    <t>TMR1</t>
+  </si>
+  <si>
+    <t>Timer 1</t>
+  </si>
+  <si>
+    <t>heartbeatTimer</t>
+  </si>
+  <si>
+    <t>Postscaler set to 2.048 seconds</t>
+  </si>
+  <si>
+    <t>Timer 1 is used as the heartbeat timer, which triggers an interrupt every second. This blinks an LED, clears the watchdog timer, and increments on time counters. Used as a 1 Hz timebase</t>
+  </si>
+  <si>
+    <t>Timer 1 period set to 61523, input frequency is 15.75 MHz, yields an IRQ rate of 1 Hz</t>
   </si>
 </sst>
 </file>
@@ -453,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3552A37-77FD-49A8-A79A-02C6EC063803}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,10 +509,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -502,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -510,38 +540,72 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added USB UART functions
</commit_message>
<xml_diff>
--- a/hdw/Logic_Board/Design_Files/Microcontroller_Peripheral_Map.xlsx
+++ b/hdw/Logic_Board/Design_Files/Microcontroller_Peripheral_Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Electronic_Display\hdw\Logic_Board\Design_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFA7EAE-7BBB-4BE9-8B95-A277318D64F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A98C3F-2A7F-4859-B59D-F804D0472282}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" xr2:uid="{B7D91EF5-14DE-4003-8C97-5F77E28EC198}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Peripheral Name</t>
   </si>
@@ -69,12 +69,6 @@
     <t>WIFI_UART</t>
   </si>
   <si>
-    <t>UART6</t>
-  </si>
-  <si>
-    <t>Universal Asynchronous Recevier Transmitter 6</t>
-  </si>
-  <si>
     <t>USB_UART</t>
   </si>
   <si>
@@ -118,6 +112,15 @@
   </si>
   <si>
     <t>Timer 1 period set to 61523, input frequency is 15.75 MHz, yields an IRQ rate of 1 Hz</t>
+  </si>
+  <si>
+    <t>UART3</t>
+  </si>
+  <si>
+    <t>Universal Asynchronous Recevier Transmitter 3</t>
+  </si>
+  <si>
+    <t>Baud rate set to 115200 bps</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -540,7 +543,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -554,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -562,50 +565,53 @@
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got basic ADC driver working
</commit_message>
<xml_diff>
--- a/hdw/Logic_Board/Design_Files/Microcontroller_Peripheral_Map.xlsx
+++ b/hdw/Logic_Board/Design_Files/Microcontroller_Peripheral_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\Electronic_Display\hdw\Logic_Board\Design_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A98C3F-2A7F-4859-B59D-F804D0472282}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDB0994-6863-4E85-9765-ABD1C496B4AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" xr2:uid="{B7D91EF5-14DE-4003-8C97-5F77E28EC198}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Peripheral Name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>WIFI_UART</t>
   </si>
   <si>
-    <t>USB_UART</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Postscaler set to 2.048 seconds</t>
   </si>
   <si>
-    <t>Timer 1 is used as the heartbeat timer, which triggers an interrupt every second. This blinks an LED, clears the watchdog timer, and increments on time counters. Used as a 1 Hz timebase</t>
-  </si>
-  <si>
     <t>Timer 1 period set to 61523, input frequency is 15.75 MHz, yields an IRQ rate of 1 Hz</t>
   </si>
   <si>
@@ -121,6 +115,45 @@
   </si>
   <si>
     <t>Baud rate set to 115200 bps</t>
+  </si>
+  <si>
+    <t>TMR3</t>
+  </si>
+  <si>
+    <t>Timer 3</t>
+  </si>
+  <si>
+    <t>Used for timebase for automatic ADC triggering</t>
+  </si>
+  <si>
+    <t>ADCTriggerTimer</t>
+  </si>
+  <si>
+    <t>DMT</t>
+  </si>
+  <si>
+    <t>Deadman timer</t>
+  </si>
+  <si>
+    <t>Resets the microcontroller if not cleared by the core timer ISR</t>
+  </si>
+  <si>
+    <t>Deadman Timer</t>
+  </si>
+  <si>
+    <t>Core Timer</t>
+  </si>
+  <si>
+    <t>CP0 integrated core timer, used for clearing the WDT and DMT</t>
+  </si>
+  <si>
+    <t>Timer 1 is used as the heartbeat timer, which triggers an interrupt every second. This blinks an LED and increments on time counters. Used as a 1 Hz timebase</t>
+  </si>
+  <si>
+    <t>Coretimer</t>
+  </si>
+  <si>
+    <t>usbUart</t>
   </si>
 </sst>
 </file>
@@ -486,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3552A37-77FD-49A8-A79A-02C6EC063803}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,7 +548,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -543,7 +576,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -557,7 +590,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -565,53 +598,95 @@
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>